<commit_message>
Step by step guidelines added
</commit_message>
<xml_diff>
--- a/Practice/semantic_similarity_sample.xlsx
+++ b/Practice/semantic_similarity_sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Haimanti Git\semantic-similarity-analysis\Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F266CE1-9C3C-4FDA-BE85-F324C2ED0137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2927E3E1-D00B-46B5-B0B4-F8A71DACC5B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A12" sqref="A12:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Semantic Similarity Sample updated
</commit_message>
<xml_diff>
--- a/Practice/semantic_similarity_sample.xlsx
+++ b/Practice/semantic_similarity_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Haimanti Git\semantic-similarity-analysis\Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2927E3E1-D00B-46B5-B0B4-F8A71DACC5B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FD45DE-7FF2-4031-BE29-17EC9646B494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,12 +112,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -147,10 +153,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -459,14 +472,14 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:C16"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -481,112 +494,112 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>0.85</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>0.7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>0.9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>0.75</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>0.95</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>0.9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>0.85</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>0.8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>0.75</v>
       </c>
     </row>

</xml_diff>